<commit_message>
Auto stash before merge of "mg_persistence" and "origin/mg_persistence"
minor updates
</commit_message>
<xml_diff>
--- a/openshift/database/dml/shersched_data.xlsx
+++ b/openshift/database/dml/shersched_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael.gabelmann/Work/_projects/jag-shuber-api/openshift/database/dml/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{37FB59F2-F6B5-DD48-9B52-6D8B1BE56C70}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{31F40620-3B45-F141-8824-8E44D4C67C2E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="640" windowWidth="31960" windowHeight="19100" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11521,8 +11521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11980,8 +11980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40FB5FAB-2770-0D4D-A97D-5A279FA0CC90}">
   <dimension ref="A1:V4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="V3" sqref="V3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11989,7 +11989,7 @@
     <col min="1" max="15" width="16.83203125" customWidth="1"/>
     <col min="16" max="18" width="19.1640625" customWidth="1"/>
     <col min="19" max="19" width="16.83203125" customWidth="1"/>
-    <col min="20" max="20" width="158" customWidth="1"/>
+    <col min="20" max="20" width="156.1640625" customWidth="1"/>
     <col min="21" max="21" width="8.83203125" customWidth="1"/>
     <col min="22" max="22" width="255.6640625" customWidth="1"/>
   </cols>

</xml_diff>